<commit_message>
Fifth commit [major corrections, back to excel again] TODO: Excel job
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>SelectionSort</t>
   </si>
@@ -28,6 +28,21 @@
   </si>
   <si>
     <t>QuickSort</t>
+  </si>
+  <si>
+    <t>1 x 100000</t>
+  </si>
+  <si>
+    <t>10 x 10000</t>
+  </si>
+  <si>
+    <t>100 x 1000</t>
+  </si>
+  <si>
+    <t>1000 x 100</t>
+  </si>
+  <si>
+    <t>10000 x 10</t>
   </si>
 </sst>
 </file>
@@ -64,7 +79,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -175,15 +190,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -212,9 +218,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -593,25 +599,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88217088"/>
-        <c:axId val="88218624"/>
+        <c:axId val="83035264"/>
+        <c:axId val="83036800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88217088"/>
+        <c:axId val="83035264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88218624"/>
+        <c:crossAx val="83036800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88218624"/>
+        <c:axId val="83036800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +625,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88217088"/>
+        <c:crossAx val="83035264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -632,7 +638,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -965,25 +971,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104367616"/>
-        <c:axId val="104369536"/>
+        <c:axId val="83067264"/>
+        <c:axId val="83068800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104367616"/>
+        <c:axId val="83067264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104369536"/>
+        <c:crossAx val="83068800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104369536"/>
+        <c:axId val="83068800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -991,7 +997,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104367616"/>
+        <c:crossAx val="83067264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1004,7 +1010,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1015,15 +1021,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1044,16 +1050,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1360,21 +1366,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:15">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1388,8 +1395,10 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="12"/>
+      <c r="O1" s="12"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -1405,8 +1414,10 @@
       <c r="E2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="7">
         <v>2000</v>
       </c>
@@ -1422,8 +1433,10 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="12"/>
+      <c r="O3" s="12"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="7">
         <v>3000</v>
       </c>
@@ -1439,8 +1452,10 @@
       <c r="E4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="12"/>
+      <c r="O4" s="12"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="7">
         <v>5000</v>
       </c>
@@ -1456,8 +1471,10 @@
       <c r="E5" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="12"/>
+      <c r="O5" s="12"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="7">
         <v>8000</v>
       </c>
@@ -1473,8 +1490,10 @@
       <c r="E6" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="12"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="7">
         <v>13000</v>
       </c>
@@ -1490,8 +1509,10 @@
       <c r="E7" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="7">
         <v>21000</v>
       </c>
@@ -1507,8 +1528,10 @@
       <c r="E8" s="6">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="7">
         <v>34000</v>
       </c>
@@ -1524,8 +1547,10 @@
       <c r="E9" s="6">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="8">
         <v>55000</v>
       </c>
@@ -1541,8 +1566,27 @@
       <c r="E10" s="10">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>0</v>
@@ -1556,9 +1600,11 @@
       <c r="E12" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="12">
+      <c r="F12" s="12"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="7">
         <v>1000</v>
       </c>
       <c r="B13" s="5">
@@ -1573,9 +1619,11 @@
       <c r="E13" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="12">
+      <c r="F13" s="12"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="7">
         <v>5000</v>
       </c>
       <c r="B14" s="5">
@@ -1590,9 +1638,11 @@
       <c r="E14" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="12">
+      <c r="F14" s="12"/>
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="7">
         <v>10000</v>
       </c>
       <c r="B15" s="5">
@@ -1607,9 +1657,11 @@
       <c r="E15" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="12">
+      <c r="F15" s="12"/>
+      <c r="O15" s="12"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="7">
         <v>50000</v>
       </c>
       <c r="B16" s="5">
@@ -1624,9 +1676,11 @@
       <c r="E16" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="12">
+      <c r="F16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="7">
         <v>100000</v>
       </c>
       <c r="B17" s="5">
@@ -1641,9 +1695,11 @@
       <c r="E17" s="6">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="12">
+      <c r="F17" s="12"/>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="7">
         <v>500000</v>
       </c>
       <c r="B18" s="5">
@@ -1658,9 +1714,11 @@
       <c r="E18" s="6">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="12">
+      <c r="F18" s="12"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="7">
         <v>1000000</v>
       </c>
       <c r="B19" s="5"/>
@@ -1669,9 +1727,11 @@
       <c r="E19" s="6">
         <v>171</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="12">
+      <c r="F19" s="12"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="8">
         <v>5000000</v>
       </c>
       <c r="B20" s="5"/>
@@ -1680,29 +1740,196 @@
       <c r="E20" s="6">
         <v>933</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="11"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="11"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="11"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5">
+        <v>18349</v>
+      </c>
+      <c r="C23" s="5">
+        <v>9046</v>
+      </c>
+      <c r="D23" s="5">
+        <v>36553</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="12"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5">
+        <v>18252</v>
+      </c>
+      <c r="C24" s="5">
+        <v>9009</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="12"/>
+      <c r="O24" s="12"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="5">
+        <v>18328</v>
+      </c>
+      <c r="C25" s="5">
+        <v>9164</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="12"/>
+      <c r="O25" s="12"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="11">
+        <v>18313</v>
+      </c>
+      <c r="C26" s="11">
+        <v>9099</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="12"/>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="11">
+        <v>18195</v>
+      </c>
+      <c r="C27" s="11">
+        <v>9076</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="11"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sixth commit [Excel Done] Release version
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>SelectionSort</t>
   </si>
@@ -59,7 +59,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,8 +78,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -143,19 +149,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -201,26 +194,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -243,7 +291,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$1</c:f>
+              <c:f>Лист1!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -257,7 +305,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$10</c:f>
+              <c:f>Лист1!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -293,36 +341,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$10</c:f>
+              <c:f>Лист1!$B$4:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>312</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>796</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2075</c:v>
+                  <c:v>2040</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5336</c:v>
+                  <c:v>5350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,7 +381,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$1</c:f>
+              <c:f>Лист1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -347,7 +395,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$10</c:f>
+              <c:f>Лист1!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -383,36 +431,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$10</c:f>
+              <c:f>Лист1!$C$4:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>156</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>421</c:v>
+                  <c:v>381</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1045</c:v>
+                  <c:v>1018</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2683</c:v>
+                  <c:v>2656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,7 +471,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$1</c:f>
+              <c:f>Лист1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,7 +485,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$10</c:f>
+              <c:f>Лист1!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -473,36 +521,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$10</c:f>
+              <c:f>Лист1!$D$4:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>124</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>265</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>639</c:v>
+                  <c:v>666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1591</c:v>
+                  <c:v>1724</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4025</c:v>
+                  <c:v>4543</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10561</c:v>
+                  <c:v>11888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,7 +561,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$E$1</c:f>
+              <c:f>Лист1!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -527,7 +575,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$10</c:f>
+              <c:f>Лист1!$A$4:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -563,7 +611,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$E$2:$E$10</c:f>
+              <c:f>Лист1!$E$4:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -577,47 +625,47 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83035264"/>
-        <c:axId val="83036800"/>
+        <c:axId val="78050816"/>
+        <c:axId val="78052352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83035264"/>
+        <c:axId val="78050816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83036800"/>
+        <c:crossAx val="78052352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83036800"/>
+        <c:axId val="78052352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +673,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83035264"/>
+        <c:crossAx val="78050816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -638,7 +686,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -657,7 +705,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$12</c:f>
+              <c:f>Лист1!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -670,61 +718,48 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
+            <c:strRef>
+              <c:f>Лист1!$A$16:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 x 100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>10 x 10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>100 x 1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>1000 x 100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>10000 x 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$13:$B$20</c:f>
+              <c:f>Лист1!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18456</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>18551</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>186</c:v>
+                  <c:v>20536</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4609</c:v>
+                  <c:v>19221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18286</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>800530</c:v>
+                  <c:v>22520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,7 +770,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$C$12</c:f>
+              <c:f>Лист1!$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -748,61 +783,48 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
+            <c:strRef>
+              <c:f>Лист1!$A$16:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 x 100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>10 x 10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>100 x 1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>1000 x 100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>10000 x 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$13:$C$20</c:f>
+              <c:f>Лист1!$C$16:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>9110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92</c:v>
+                  <c:v>9420</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2214</c:v>
+                  <c:v>8989</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>355205</c:v>
+                  <c:v>8219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -813,7 +835,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$12</c:f>
+              <c:f>Лист1!$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -826,61 +848,48 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
+            <c:strRef>
+              <c:f>Лист1!$A$16:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 x 100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>10 x 10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>100 x 1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>1000 x 100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>10000 x 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$13:$D$20</c:f>
+              <c:f>Лист1!$D$16:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124</c:v>
+                  <c:v>25384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>389</c:v>
+                  <c:v>18596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8944</c:v>
+                  <c:v>18168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35850</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1507350</c:v>
+                  <c:v>17920</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -891,7 +900,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$E$12</c:f>
+              <c:f>Лист1!$E$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -904,92 +913,72 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>Лист1!$A$13:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
+            <c:strRef>
+              <c:f>Лист1!$A$16:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1 x 100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>10 x 10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>100 x 1000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50000</c:v>
+                  <c:v>1000 x 100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>10000 x 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$E$13:$E$20</c:f>
+              <c:f>Лист1!$E$16:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>933</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83067264"/>
-        <c:axId val="83068800"/>
+        <c:axId val="54474240"/>
+        <c:axId val="54475776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83067264"/>
+        <c:axId val="54474240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83068800"/>
+        <c:crossAx val="54475776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83068800"/>
+        <c:axId val="54475776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +986,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83067264"/>
+        <c:crossAx val="54474240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1010,7 +999,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1022,13 +1011,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1050,20 +1039,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1366,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1379,557 +1368,704 @@
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4">
+      <c r="F3" s="4"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="11"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="21">
         <v>1000</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B4" s="24">
+        <v>3</v>
+      </c>
+      <c r="C4" s="24">
+        <v>1</v>
+      </c>
+      <c r="D4" s="24">
+        <v>4</v>
+      </c>
+      <c r="E4" s="25">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="F4" s="10"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="11"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="22">
+        <v>2000</v>
+      </c>
+      <c r="B5" s="24">
+        <v>8</v>
+      </c>
+      <c r="C5" s="24">
+        <v>3</v>
+      </c>
+      <c r="D5" s="24">
+        <v>15</v>
+      </c>
+      <c r="E5" s="25">
         <v>0</v>
       </c>
-      <c r="D2" s="5">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="F5" s="10"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="22">
+        <v>3000</v>
+      </c>
+      <c r="B6" s="24">
+        <v>15</v>
+      </c>
+      <c r="C6" s="24">
+        <v>8</v>
+      </c>
+      <c r="D6" s="24">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25">
         <v>0</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="7">
-        <v>2000</v>
-      </c>
-      <c r="B3" s="5">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="F6" s="10"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="22">
+        <v>5000</v>
+      </c>
+      <c r="B7" s="24">
+        <v>43</v>
+      </c>
+      <c r="C7" s="24">
+        <v>21</v>
+      </c>
+      <c r="D7" s="24">
+        <v>97</v>
+      </c>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="22">
+        <v>8000</v>
+      </c>
+      <c r="B8" s="24">
+        <v>109</v>
+      </c>
+      <c r="C8" s="24">
+        <v>54</v>
+      </c>
+      <c r="D8" s="24">
+        <v>248</v>
+      </c>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="11"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="22">
+        <v>13000</v>
+      </c>
+      <c r="B9" s="24">
+        <v>293</v>
+      </c>
+      <c r="C9" s="24">
+        <v>144</v>
+      </c>
+      <c r="D9" s="24">
+        <v>666</v>
+      </c>
+      <c r="E9" s="25">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="11"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="22">
+        <v>21000</v>
+      </c>
+      <c r="B10" s="24">
+        <v>771</v>
+      </c>
+      <c r="C10" s="24">
+        <v>381</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1724</v>
+      </c>
+      <c r="E10" s="25">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="22">
+        <v>34000</v>
+      </c>
+      <c r="B11" s="24">
+        <v>2040</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1018</v>
+      </c>
+      <c r="D11" s="24">
+        <v>4543</v>
+      </c>
+      <c r="E11" s="25">
+        <v>5</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="23">
+        <v>55000</v>
+      </c>
+      <c r="B12" s="26">
+        <v>5350</v>
+      </c>
+      <c r="C12" s="26">
+        <v>2656</v>
+      </c>
+      <c r="D12" s="26">
+        <v>11888</v>
+      </c>
+      <c r="E12" s="27">
+        <v>8</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="11"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="24">
+        <v>18456</v>
+      </c>
+      <c r="C16" s="24">
+        <v>9110</v>
+      </c>
+      <c r="D16" s="24">
+        <v>40802</v>
+      </c>
+      <c r="E16" s="25">
         <v>15</v>
       </c>
-      <c r="D3" s="5">
-        <v>31</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="O3" s="12"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="7">
-        <v>3000</v>
-      </c>
-      <c r="B4" s="5">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5">
-        <v>62</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B5" s="5">
-        <v>62</v>
-      </c>
-      <c r="C5" s="5">
-        <v>47</v>
-      </c>
-      <c r="D5" s="11">
-        <v>124</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="7">
-        <v>8000</v>
-      </c>
-      <c r="B6" s="5">
-        <v>125</v>
-      </c>
-      <c r="C6" s="5">
-        <v>62</v>
-      </c>
-      <c r="D6" s="11">
-        <v>265</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="7">
-        <v>13000</v>
-      </c>
-      <c r="B7" s="5">
-        <v>312</v>
-      </c>
-      <c r="C7" s="5">
-        <v>156</v>
-      </c>
-      <c r="D7" s="11">
-        <v>639</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="7">
-        <v>21000</v>
-      </c>
-      <c r="B8" s="5">
-        <v>796</v>
-      </c>
-      <c r="C8" s="5">
-        <v>421</v>
-      </c>
-      <c r="D8" s="11">
-        <v>1591</v>
-      </c>
-      <c r="E8" s="6">
-        <v>16</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="7">
-        <v>34000</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2075</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1045</v>
-      </c>
-      <c r="D9" s="11">
-        <v>4025</v>
-      </c>
-      <c r="E9" s="6">
-        <v>16</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="8">
-        <v>55000</v>
-      </c>
-      <c r="B10" s="9">
-        <v>5336</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2683</v>
-      </c>
-      <c r="D10" s="9">
-        <v>10561</v>
-      </c>
-      <c r="E10" s="10">
-        <v>31</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="7">
-        <v>1000</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="7">
-        <v>5000</v>
-      </c>
-      <c r="B14" s="5">
-        <v>42</v>
-      </c>
-      <c r="C14" s="5">
-        <v>38</v>
-      </c>
-      <c r="D14" s="11">
-        <v>124</v>
-      </c>
-      <c r="E14" s="6">
-        <v>3</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="7">
-        <v>10000</v>
-      </c>
-      <c r="B15" s="5">
-        <v>186</v>
-      </c>
-      <c r="C15" s="5">
-        <v>92</v>
-      </c>
-      <c r="D15" s="11">
-        <v>389</v>
-      </c>
-      <c r="E15" s="6">
-        <v>4</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="7">
-        <v>50000</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4609</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2214</v>
-      </c>
-      <c r="D16" s="11">
-        <v>8944</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="F16" s="10"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="11"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="24">
+        <v>18551</v>
+      </c>
+      <c r="C17" s="24">
+        <v>9110</v>
+      </c>
+      <c r="D17" s="24">
+        <v>25384</v>
+      </c>
+      <c r="E17" s="25">
+        <v>15</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="7">
-        <v>100000</v>
-      </c>
-      <c r="B17" s="5">
-        <v>18286</v>
-      </c>
-      <c r="C17" s="5">
-        <v>8995</v>
-      </c>
-      <c r="D17" s="11">
-        <v>35850</v>
-      </c>
-      <c r="E17" s="6">
-        <v>48</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="O17" s="12"/>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="7">
-        <v>500000</v>
-      </c>
-      <c r="B18" s="5">
-        <v>800530</v>
-      </c>
-      <c r="C18" s="5">
-        <v>355205</v>
-      </c>
-      <c r="D18" s="11">
-        <v>1507350</v>
-      </c>
-      <c r="E18" s="6">
-        <v>87</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="O18" s="12"/>
+      <c r="B18" s="24">
+        <v>20536</v>
+      </c>
+      <c r="C18" s="24">
+        <v>9420</v>
+      </c>
+      <c r="D18" s="24">
+        <v>18596</v>
+      </c>
+      <c r="E18" s="25">
+        <v>14</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="7">
-        <v>1000000</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6">
-        <v>171</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="O19" s="12"/>
+      <c r="A19" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="24">
+        <v>19221</v>
+      </c>
+      <c r="C19" s="24">
+        <v>8989</v>
+      </c>
+      <c r="D19" s="24">
+        <v>18168</v>
+      </c>
+      <c r="E19" s="25">
+        <v>15</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="11"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="8">
-        <v>5000000</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6">
-        <v>933</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="O20" s="12"/>
+      <c r="A20" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="24">
+        <v>22520</v>
+      </c>
+      <c r="C20" s="24">
+        <v>8219</v>
+      </c>
+      <c r="D20" s="24">
+        <v>17920</v>
+      </c>
+      <c r="E20" s="25">
+        <v>14</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="12"/>
-      <c r="O22" s="12"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="5">
-        <v>18349</v>
-      </c>
-      <c r="C23" s="5">
-        <v>9046</v>
-      </c>
-      <c r="D23" s="5">
-        <v>36553</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="12"/>
-      <c r="O23" s="12"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="11"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="5">
-        <v>18252</v>
-      </c>
-      <c r="C24" s="5">
-        <v>9009</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="12"/>
-      <c r="O24" s="12"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="5">
-        <v>18328</v>
-      </c>
-      <c r="C25" s="5">
-        <v>9164</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="12"/>
-      <c r="O25" s="12"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="11">
-        <v>18313</v>
-      </c>
-      <c r="C26" s="11">
-        <v>9099</v>
-      </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="12"/>
-      <c r="O26" s="12"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="11">
-        <v>18195</v>
-      </c>
-      <c r="C27" s="11">
-        <v>9076</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="12"/>
-      <c r="O27" s="12"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="11"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="11"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="11"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="8:15">
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>